<commit_message>
Version semi estable, faltan completar variables
</commit_message>
<xml_diff>
--- a/6.Cadena_de_valor.xlsx
+++ b/6.Cadena_de_valor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos D\Gobernación\APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DE6E43-1DA1-41DC-893C-9FE6249C049D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC0F003-B1B0-4316-B780-1B8666FBEE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -761,13 +761,13 @@
     <t>Medido a través de</t>
   </si>
   <si>
-    <t>Firma del Secretario/Jefe de Oficina/Dependencia</t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
     <t>OTROS (Especificar cual) (Coop. Internacional)</t>
+  </si>
+  <si>
+    <t>Firma del Secretario(a)/Jefe de oficina</t>
   </si>
 </sst>
 </file>
@@ -2011,6 +2011,111 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="23" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="23" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2029,21 +2134,9 @@
     <xf numFmtId="0" fontId="25" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2062,86 +2155,14 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2177,27 +2198,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7025,7 +7025,7 @@
   </sheetPr>
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="62" zoomScaleNormal="85" zoomScaleSheetLayoutView="62" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="62" zoomScaleNormal="85" zoomScaleSheetLayoutView="62" workbookViewId="0">
       <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
@@ -7053,21 +7053,21 @@
   <sheetData>
     <row r="1" spans="1:23" s="53" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="97"/>
-      <c r="B1" s="123" t="s">
+      <c r="B1" s="158" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="124"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
+      <c r="I1" s="158"/>
+      <c r="J1" s="158"/>
+      <c r="K1" s="158"/>
+      <c r="L1" s="158"/>
+      <c r="M1" s="158"/>
+      <c r="N1" s="159"/>
       <c r="O1" s="107" t="s">
         <v>196</v>
       </c>
@@ -7081,25 +7081,25 @@
       <c r="A2" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="179"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="181"/>
-      <c r="F2" s="144" t="s">
+      <c r="B2" s="171"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="155" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="144"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="147" t="s">
+      <c r="G2" s="155"/>
+      <c r="H2" s="166"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="137" t="s">
         <v>199</v>
       </c>
-      <c r="K2" s="149"/>
-      <c r="L2" s="150"/>
-      <c r="M2" s="153" t="s">
+      <c r="K2" s="139"/>
+      <c r="L2" s="140"/>
+      <c r="M2" s="143" t="s">
         <v>195</v>
       </c>
-      <c r="N2" s="182"/>
+      <c r="N2" s="145"/>
       <c r="O2" s="108" t="s">
         <v>220</v>
       </c>
@@ -7113,19 +7113,19 @@
       <c r="A3" s="101" t="s">
         <v>200</v>
       </c>
-      <c r="B3" s="140"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="138"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="151"/>
-      <c r="L3" s="152"/>
-      <c r="M3" s="154"/>
-      <c r="N3" s="183"/>
+      <c r="B3" s="149"/>
+      <c r="C3" s="150"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="155"/>
+      <c r="H3" s="168"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="141"/>
+      <c r="L3" s="142"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="146"/>
       <c r="O3" s="108" t="s">
         <v>221</v>
       </c>
@@ -7136,27 +7136,27 @@
       <c r="T3" s="103"/>
     </row>
     <row r="4" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="163"/>
-      <c r="B4" s="161"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="162"/>
-      <c r="H4" s="160"/>
-      <c r="I4" s="161"/>
-      <c r="J4" s="161"/>
-      <c r="K4" s="161"/>
-      <c r="L4" s="162"/>
+      <c r="A4" s="131"/>
+      <c r="B4" s="129"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="130"/>
       <c r="M4" s="75"/>
       <c r="N4" s="75"/>
       <c r="O4" s="75"/>
       <c r="P4" s="110"/>
-      <c r="Q4" s="155" t="s">
+      <c r="Q4" s="147" t="s">
         <v>208</v>
       </c>
-      <c r="R4" s="156"/>
-      <c r="S4" s="156"/>
+      <c r="R4" s="148"/>
+      <c r="S4" s="148"/>
       <c r="T4" s="104"/>
     </row>
     <row r="5" spans="1:23" ht="81" customHeight="1" x14ac:dyDescent="0.25">
@@ -7215,21 +7215,21 @@
         <v>210</v>
       </c>
       <c r="S5" s="76" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T5" s="120" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:23" s="57" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="126"/>
-      <c r="B6" s="129"/>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
-      <c r="E6" s="132" t="s">
+      <c r="A6" s="161"/>
+      <c r="B6" s="156"/>
+      <c r="C6" s="156"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="152" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="129"/>
+      <c r="F6" s="156"/>
       <c r="G6" s="72">
         <v>0</v>
       </c>
@@ -7248,19 +7248,19 @@
       <c r="Q6" s="77"/>
       <c r="R6" s="77"/>
       <c r="S6" s="77"/>
-      <c r="T6" s="145">
+      <c r="T6" s="135">
         <f>+P6+P7</f>
         <v>0</v>
       </c>
       <c r="W6" s="74"/>
     </row>
     <row r="7" spans="1:23" s="57" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="127"/>
-      <c r="B7" s="130"/>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
-      <c r="E7" s="133"/>
-      <c r="F7" s="131"/>
+      <c r="A7" s="162"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="164"/>
+      <c r="D7" s="164"/>
+      <c r="E7" s="154"/>
+      <c r="F7" s="157"/>
       <c r="G7" s="72">
         <v>1</v>
       </c>
@@ -7279,18 +7279,18 @@
       <c r="Q7" s="77"/>
       <c r="R7" s="77"/>
       <c r="S7" s="77"/>
-      <c r="T7" s="146"/>
+      <c r="T7" s="136"/>
       <c r="W7" s="74"/>
     </row>
     <row r="8" spans="1:23" s="57" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="127"/>
-      <c r="B8" s="130"/>
-      <c r="C8" s="130"/>
-      <c r="D8" s="130"/>
-      <c r="E8" s="129" t="s">
+      <c r="A8" s="162"/>
+      <c r="B8" s="164"/>
+      <c r="C8" s="164"/>
+      <c r="D8" s="164"/>
+      <c r="E8" s="156" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="129"/>
+      <c r="F8" s="156"/>
       <c r="G8" s="72">
         <v>0</v>
       </c>
@@ -7309,19 +7309,19 @@
       <c r="Q8" s="77"/>
       <c r="R8" s="77"/>
       <c r="S8" s="77"/>
-      <c r="T8" s="145">
+      <c r="T8" s="135">
         <f t="shared" ref="T8" si="1">+P8+P9</f>
         <v>0</v>
       </c>
       <c r="W8" s="74"/>
     </row>
     <row r="9" spans="1:23" s="57" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="128"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="131"/>
+      <c r="A9" s="163"/>
+      <c r="B9" s="157"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="157"/>
+      <c r="E9" s="157"/>
+      <c r="F9" s="157"/>
       <c r="G9" s="67">
         <v>1</v>
       </c>
@@ -7340,20 +7340,20 @@
       <c r="Q9" s="77"/>
       <c r="R9" s="77"/>
       <c r="S9" s="77"/>
-      <c r="T9" s="146"/>
+      <c r="T9" s="136"/>
       <c r="U9" s="73"/>
       <c r="V9" s="73"/>
       <c r="W9" s="74"/>
     </row>
     <row r="10" spans="1:23" s="57" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="134"/>
-      <c r="B10" s="125"/>
-      <c r="C10" s="132"/>
-      <c r="D10" s="132"/>
-      <c r="E10" s="139" t="s">
+      <c r="A10" s="165"/>
+      <c r="B10" s="160"/>
+      <c r="C10" s="152"/>
+      <c r="D10" s="152"/>
+      <c r="E10" s="170" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="139"/>
+      <c r="F10" s="170"/>
       <c r="G10" s="67">
         <v>0</v>
       </c>
@@ -7372,19 +7372,19 @@
       <c r="Q10" s="77"/>
       <c r="R10" s="77"/>
       <c r="S10" s="77"/>
-      <c r="T10" s="145">
+      <c r="T10" s="135">
         <f t="shared" ref="T10" si="2">+P10+P11</f>
         <v>0</v>
       </c>
       <c r="W10" s="74"/>
     </row>
     <row r="11" spans="1:23" s="57" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="134"/>
-      <c r="B11" s="125"/>
-      <c r="C11" s="143"/>
-      <c r="D11" s="143"/>
-      <c r="E11" s="139"/>
-      <c r="F11" s="139"/>
+      <c r="A11" s="165"/>
+      <c r="B11" s="160"/>
+      <c r="C11" s="153"/>
+      <c r="D11" s="153"/>
+      <c r="E11" s="170"/>
+      <c r="F11" s="170"/>
       <c r="G11" s="67">
         <v>1</v>
       </c>
@@ -7403,18 +7403,18 @@
       <c r="Q11" s="77"/>
       <c r="R11" s="77"/>
       <c r="S11" s="77"/>
-      <c r="T11" s="146"/>
+      <c r="T11" s="136"/>
       <c r="W11" s="74"/>
     </row>
     <row r="12" spans="1:23" s="57" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="134"/>
-      <c r="B12" s="125"/>
-      <c r="C12" s="143"/>
-      <c r="D12" s="143"/>
-      <c r="E12" s="139" t="s">
+      <c r="A12" s="165"/>
+      <c r="B12" s="160"/>
+      <c r="C12" s="153"/>
+      <c r="D12" s="153"/>
+      <c r="E12" s="170" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="139"/>
+      <c r="F12" s="170"/>
       <c r="G12" s="67">
         <v>0</v>
       </c>
@@ -7433,19 +7433,19 @@
       <c r="Q12" s="77"/>
       <c r="R12" s="77"/>
       <c r="S12" s="77"/>
-      <c r="T12" s="145">
+      <c r="T12" s="135">
         <f t="shared" ref="T12" si="3">+P12+P13</f>
         <v>0</v>
       </c>
       <c r="W12" s="74"/>
     </row>
     <row r="13" spans="1:23" s="57" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="134"/>
-      <c r="B13" s="125"/>
-      <c r="C13" s="133"/>
-      <c r="D13" s="133"/>
-      <c r="E13" s="139"/>
-      <c r="F13" s="139"/>
+      <c r="A13" s="165"/>
+      <c r="B13" s="160"/>
+      <c r="C13" s="154"/>
+      <c r="D13" s="154"/>
+      <c r="E13" s="170"/>
+      <c r="F13" s="170"/>
       <c r="G13" s="67">
         <v>1</v>
       </c>
@@ -7464,18 +7464,18 @@
       <c r="Q13" s="77"/>
       <c r="R13" s="77"/>
       <c r="S13" s="77"/>
-      <c r="T13" s="146"/>
+      <c r="T13" s="136"/>
       <c r="W13" s="74"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="164"/>
-      <c r="B14" s="165"/>
-      <c r="C14" s="165"/>
-      <c r="D14" s="165"/>
-      <c r="E14" s="165"/>
-      <c r="F14" s="165"/>
-      <c r="G14" s="165"/>
-      <c r="H14" s="166"/>
+      <c r="A14" s="132"/>
+      <c r="B14" s="133"/>
+      <c r="C14" s="133"/>
+      <c r="D14" s="133"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
+      <c r="G14" s="133"/>
+      <c r="H14" s="134"/>
       <c r="I14" s="105"/>
       <c r="J14" s="106">
         <f>SUM(J6:J13)</f>
@@ -7530,8 +7530,8 @@
     </row>
     <row r="16" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="157"/>
-      <c r="B17" s="157"/>
+      <c r="A17" s="123"/>
+      <c r="B17" s="123"/>
       <c r="F17" s="80" t="s">
         <v>205</v>
       </c>
@@ -7592,8 +7592,8 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="157"/>
-      <c r="B18" s="157"/>
+      <c r="A18" s="123"/>
+      <c r="B18" s="123"/>
       <c r="C18" s="121"/>
       <c r="F18" s="80" t="s">
         <v>206</v>
@@ -7655,8 +7655,8 @@
       </c>
     </row>
     <row r="19" spans="1:20" s="114" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="158"/>
-      <c r="B19" s="158"/>
+      <c r="A19" s="124"/>
+      <c r="B19" s="124"/>
       <c r="C19" s="121"/>
       <c r="F19" s="115" t="s">
         <v>194</v>
@@ -7716,40 +7716,20 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="159" t="s">
+      <c r="A20" s="125" t="s">
+        <v>225</v>
+      </c>
+      <c r="B20" s="125"/>
+      <c r="C20" s="121"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="126" t="s">
         <v>223</v>
       </c>
-      <c r="B20" s="159"/>
-      <c r="C20" s="121"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="184" t="s">
-        <v>224</v>
-      </c>
-      <c r="B21" s="185"/>
+      <c r="B21" s="127"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A17:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="T12:T13"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="F2:G3"/>
-    <mergeCell ref="F8:F9"/>
     <mergeCell ref="B1:N1"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="A6:A9"/>
@@ -7766,6 +7746,26 @@
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="F2:G3"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="T12:T13"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="A17:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A14:H14"/>
   </mergeCells>
   <phoneticPr fontId="30" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -7806,14 +7806,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="167"/>
-      <c r="B1" s="168"/>
-      <c r="C1" s="168"/>
-      <c r="D1" s="168"/>
-      <c r="E1" s="168"/>
-      <c r="F1" s="168"/>
-      <c r="G1" s="168"/>
-      <c r="H1" s="168"/>
+      <c r="A1" s="174"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
+      <c r="H1" s="175"/>
     </row>
     <row r="2" spans="1:21" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
@@ -8012,8 +8012,8 @@
       <c r="D12" s="62"/>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
-      <c r="G12" s="169"/>
-      <c r="H12" s="170"/>
+      <c r="G12" s="176"/>
+      <c r="H12" s="177"/>
       <c r="I12" s="62"/>
       <c r="J12" s="62"/>
       <c r="K12" s="62"/>
@@ -8214,18 +8214,18 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="174" t="s">
+      <c r="A2" s="181" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="183" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="178"/>
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="185"/>
     </row>
     <row r="3" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="175"/>
+      <c r="A3" s="182"/>
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
@@ -8240,7 +8240,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="171" t="s">
+      <c r="A4" s="178" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -8253,7 +8253,7 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="172"/>
+      <c r="A5" s="179"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
         <v>25</v>
@@ -8262,7 +8262,7 @@
       <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="173"/>
+      <c r="A6" s="180"/>
       <c r="B6" s="12"/>
       <c r="C6" s="13" t="s">
         <v>26</v>
@@ -8271,7 +8271,7 @@
       <c r="E6" s="14"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="171" t="s">
+      <c r="A7" s="178" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -8284,7 +8284,7 @@
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="172"/>
+      <c r="A8" s="179"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10" t="s">
         <v>25</v>
@@ -8293,7 +8293,7 @@
       <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="173"/>
+      <c r="A9" s="180"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13" t="s">
         <v>26</v>
@@ -8302,7 +8302,7 @@
       <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="171" t="s">
+      <c r="A10" s="178" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -8317,7 +8317,7 @@
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="172"/>
+      <c r="A11" s="179"/>
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
@@ -8330,7 +8330,7 @@
       <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="173"/>
+      <c r="A12" s="180"/>
       <c r="B12" s="12" t="s">
         <v>28</v>
       </c>
@@ -8606,7 +8606,7 @@
       <c r="E39" s="28"/>
     </row>
     <row r="40" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="171" t="s">
+      <c r="A40" s="178" t="s">
         <v>69</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -8621,7 +8621,7 @@
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="172"/>
+      <c r="A41" s="179"/>
       <c r="B41" s="9"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10" t="s">
@@ -8630,7 +8630,7 @@
       <c r="E41" s="11"/>
     </row>
     <row r="42" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="173"/>
+      <c r="A42" s="180"/>
       <c r="B42" s="12" t="s">
         <v>28</v>
       </c>
@@ -8645,7 +8645,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="171" t="s">
+      <c r="A43" s="178" t="s">
         <v>74</v>
       </c>
       <c r="B43" s="6" t="s">
@@ -8662,7 +8662,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="172"/>
+      <c r="A44" s="179"/>
       <c r="B44" s="9" t="s">
         <v>35</v>
       </c>
@@ -8675,7 +8675,7 @@
       <c r="E44" s="11"/>
     </row>
     <row r="45" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="172"/>
+      <c r="A45" s="179"/>
       <c r="B45" s="9"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
@@ -8684,7 +8684,7 @@
       <c r="E45" s="11"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="172"/>
+      <c r="A46" s="179"/>
       <c r="B46" s="9"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
@@ -8693,7 +8693,7 @@
       <c r="E46" s="11"/>
     </row>
     <row r="47" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="172"/>
+      <c r="A47" s="179"/>
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10" t="s">
@@ -8702,7 +8702,7 @@
       <c r="E47" s="11"/>
     </row>
     <row r="48" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="172"/>
+      <c r="A48" s="179"/>
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
       <c r="D48" s="10" t="s">
@@ -8711,7 +8711,7 @@
       <c r="E48" s="11"/>
     </row>
     <row r="49" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="173"/>
+      <c r="A49" s="180"/>
       <c r="B49" s="12"/>
       <c r="C49" s="13"/>
       <c r="D49" s="13" t="s">
@@ -8735,7 +8735,7 @@
       <c r="E50" s="30"/>
     </row>
     <row r="51" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="171" t="s">
+      <c r="A51" s="178" t="s">
         <v>85</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -8750,7 +8750,7 @@
       <c r="E51" s="31"/>
     </row>
     <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="172"/>
+      <c r="A52" s="179"/>
       <c r="B52" s="9"/>
       <c r="C52" s="10"/>
       <c r="D52" s="10" t="s">
@@ -8759,7 +8759,7 @@
       <c r="E52" s="32"/>
     </row>
     <row r="53" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="173"/>
+      <c r="A53" s="180"/>
       <c r="B53" s="33"/>
       <c r="C53" s="13"/>
       <c r="D53" s="13" t="s">
@@ -8768,7 +8768,7 @@
       <c r="E53" s="14"/>
     </row>
     <row r="54" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="171" t="s">
+      <c r="A54" s="178" t="s">
         <v>90</v>
       </c>
       <c r="B54" s="6" t="s">
@@ -8783,7 +8783,7 @@
       <c r="E54" s="8"/>
     </row>
     <row r="55" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="173"/>
+      <c r="A55" s="180"/>
       <c r="B55" s="33"/>
       <c r="C55" s="13" t="s">
         <v>92</v>
@@ -8794,7 +8794,7 @@
       <c r="E55" s="15"/>
     </row>
     <row r="56" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="171" t="s">
+      <c r="A56" s="178" t="s">
         <v>94</v>
       </c>
       <c r="B56" s="6" t="s">
@@ -8809,7 +8809,7 @@
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="172"/>
+      <c r="A57" s="179"/>
       <c r="B57" s="34"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10" t="s">
@@ -8818,7 +8818,7 @@
       <c r="E57" s="11"/>
     </row>
     <row r="58" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A58" s="172"/>
+      <c r="A58" s="179"/>
       <c r="B58" s="34"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10" t="s">
@@ -8827,7 +8827,7 @@
       <c r="E58" s="11"/>
     </row>
     <row r="59" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A59" s="172"/>
+      <c r="A59" s="179"/>
       <c r="B59" s="34"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10" t="s">
@@ -8836,7 +8836,7 @@
       <c r="E59" s="11"/>
     </row>
     <row r="60" spans="1:5" ht="47.25" x14ac:dyDescent="0.3">
-      <c r="A60" s="172"/>
+      <c r="A60" s="179"/>
       <c r="B60" s="34"/>
       <c r="C60" s="10" t="s">
         <v>99</v>
@@ -8847,7 +8847,7 @@
       <c r="E60" s="11"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="172"/>
+      <c r="A61" s="179"/>
       <c r="B61" s="34"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
@@ -8856,7 +8856,7 @@
       <c r="E61" s="11"/>
     </row>
     <row r="62" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A62" s="172"/>
+      <c r="A62" s="179"/>
       <c r="B62" s="34"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10" t="s">
@@ -8865,7 +8865,7 @@
       <c r="E62" s="11"/>
     </row>
     <row r="63" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A63" s="172"/>
+      <c r="A63" s="179"/>
       <c r="B63" s="34"/>
       <c r="C63" s="10" t="s">
         <v>83</v>
@@ -8876,7 +8876,7 @@
       <c r="E63" s="11"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="172"/>
+      <c r="A64" s="179"/>
       <c r="B64" s="34"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="s">
@@ -8885,7 +8885,7 @@
       <c r="E64" s="11"/>
     </row>
     <row r="65" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A65" s="172"/>
+      <c r="A65" s="179"/>
       <c r="B65" s="34"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10" t="s">
@@ -8894,7 +8894,7 @@
       <c r="E65" s="11"/>
     </row>
     <row r="66" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A66" s="172"/>
+      <c r="A66" s="179"/>
       <c r="B66" s="34"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10" t="s">
@@ -8903,7 +8903,7 @@
       <c r="E66" s="11"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="172"/>
+      <c r="A67" s="179"/>
       <c r="B67" s="34"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
@@ -8912,7 +8912,7 @@
       <c r="E67" s="11"/>
     </row>
     <row r="68" spans="1:5" ht="47.25" x14ac:dyDescent="0.3">
-      <c r="A68" s="172"/>
+      <c r="A68" s="179"/>
       <c r="B68" s="34"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10" t="s">
@@ -8921,7 +8921,7 @@
       <c r="E68" s="11"/>
     </row>
     <row r="69" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A69" s="172"/>
+      <c r="A69" s="179"/>
       <c r="B69" s="34"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10" t="s">
@@ -8930,7 +8930,7 @@
       <c r="E69" s="11"/>
     </row>
     <row r="70" spans="1:5" ht="63" x14ac:dyDescent="0.3">
-      <c r="A70" s="172"/>
+      <c r="A70" s="179"/>
       <c r="B70" s="34"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
@@ -8939,7 +8939,7 @@
       <c r="E70" s="11"/>
     </row>
     <row r="71" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A71" s="172"/>
+      <c r="A71" s="179"/>
       <c r="B71" s="34"/>
       <c r="C71" s="10" t="s">
         <v>92</v>
@@ -8950,7 +8950,7 @@
       <c r="E71" s="11"/>
     </row>
     <row r="72" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A72" s="172"/>
+      <c r="A72" s="179"/>
       <c r="B72" s="34"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10" t="s">
@@ -8959,7 +8959,7 @@
       <c r="E72" s="11"/>
     </row>
     <row r="73" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A73" s="172"/>
+      <c r="A73" s="179"/>
       <c r="B73" s="34"/>
       <c r="C73" s="10"/>
       <c r="D73" s="10" t="s">
@@ -8968,7 +8968,7 @@
       <c r="E73" s="11"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="172"/>
+      <c r="A74" s="179"/>
       <c r="B74" s="34"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10" t="s">
@@ -8977,7 +8977,7 @@
       <c r="E74" s="11"/>
     </row>
     <row r="75" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="173"/>
+      <c r="A75" s="180"/>
       <c r="B75" s="33"/>
       <c r="C75" s="13"/>
       <c r="D75" s="13" t="s">
@@ -8986,7 +8986,7 @@
       <c r="E75" s="14"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="171" t="s">
+      <c r="A76" s="178" t="s">
         <v>116</v>
       </c>
       <c r="B76" s="35" t="s">
@@ -9001,7 +9001,7 @@
       <c r="E76" s="8"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="172"/>
+      <c r="A77" s="179"/>
       <c r="B77" s="34"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10" t="s">
@@ -9010,7 +9010,7 @@
       <c r="E77" s="11"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="172"/>
+      <c r="A78" s="179"/>
       <c r="B78" s="36" t="s">
         <v>119</v>
       </c>
@@ -9023,7 +9023,7 @@
       <c r="E78" s="11"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="172"/>
+      <c r="A79" s="179"/>
       <c r="B79" s="34"/>
       <c r="C79" s="10"/>
       <c r="D79" s="10" t="s">
@@ -9032,7 +9032,7 @@
       <c r="E79" s="11"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="172"/>
+      <c r="A80" s="179"/>
       <c r="B80" s="34"/>
       <c r="C80" s="10"/>
       <c r="D80" s="10" t="s">
@@ -9041,7 +9041,7 @@
       <c r="E80" s="11"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="172"/>
+      <c r="A81" s="179"/>
       <c r="B81" s="34"/>
       <c r="C81" s="10"/>
       <c r="D81" s="10" t="s">
@@ -9050,7 +9050,7 @@
       <c r="E81" s="11"/>
     </row>
     <row r="82" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A82" s="172"/>
+      <c r="A82" s="179"/>
       <c r="B82" s="34"/>
       <c r="C82" s="10" t="s">
         <v>125</v>
@@ -9061,7 +9061,7 @@
       <c r="E82" s="11"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="172"/>
+      <c r="A83" s="179"/>
       <c r="B83" s="34"/>
       <c r="C83" s="10"/>
       <c r="D83" s="10" t="s">
@@ -9070,7 +9070,7 @@
       <c r="E83" s="11"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="172"/>
+      <c r="A84" s="179"/>
       <c r="B84" s="34"/>
       <c r="C84" s="10" t="s">
         <v>128</v>
@@ -9081,7 +9081,7 @@
       <c r="E84" s="11"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="172"/>
+      <c r="A85" s="179"/>
       <c r="B85" s="34"/>
       <c r="C85" s="10"/>
       <c r="D85" s="10" t="s">
@@ -9090,7 +9090,7 @@
       <c r="E85" s="11"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" s="172"/>
+      <c r="A86" s="179"/>
       <c r="B86" s="34"/>
       <c r="C86" s="10"/>
       <c r="D86" s="10" t="s">
@@ -9099,7 +9099,7 @@
       <c r="E86" s="11"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" s="172"/>
+      <c r="A87" s="179"/>
       <c r="B87" s="34"/>
       <c r="C87" s="10"/>
       <c r="D87" s="10" t="s">
@@ -9108,7 +9108,7 @@
       <c r="E87" s="11"/>
     </row>
     <row r="88" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A88" s="172"/>
+      <c r="A88" s="179"/>
       <c r="B88" s="34"/>
       <c r="C88" s="10" t="s">
         <v>133</v>
@@ -9119,7 +9119,7 @@
       <c r="E88" s="11"/>
     </row>
     <row r="89" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A89" s="172"/>
+      <c r="A89" s="179"/>
       <c r="B89" s="34"/>
       <c r="C89" s="10"/>
       <c r="D89" s="10" t="s">
@@ -9128,7 +9128,7 @@
       <c r="E89" s="11"/>
     </row>
     <row r="90" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A90" s="172"/>
+      <c r="A90" s="179"/>
       <c r="B90" s="34"/>
       <c r="C90" s="10"/>
       <c r="D90" s="10" t="s">
@@ -9137,7 +9137,7 @@
       <c r="E90" s="11"/>
     </row>
     <row r="91" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A91" s="172"/>
+      <c r="A91" s="179"/>
       <c r="B91" s="34"/>
       <c r="C91" s="10" t="s">
         <v>137</v>
@@ -9146,7 +9146,7 @@
       <c r="E91" s="11"/>
     </row>
     <row r="92" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A92" s="172"/>
+      <c r="A92" s="179"/>
       <c r="B92" s="34"/>
       <c r="C92" s="10" t="s">
         <v>138</v>
@@ -9155,7 +9155,7 @@
       <c r="E92" s="11"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A93" s="172"/>
+      <c r="A93" s="179"/>
       <c r="B93" s="34"/>
       <c r="C93" s="10" t="s">
         <v>139</v>
@@ -9164,7 +9164,7 @@
       <c r="E93" s="11"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A94" s="172"/>
+      <c r="A94" s="179"/>
       <c r="B94" s="34"/>
       <c r="C94" s="10" t="s">
         <v>140</v>
@@ -9173,7 +9173,7 @@
       <c r="E94" s="11"/>
     </row>
     <row r="95" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A95" s="172"/>
+      <c r="A95" s="179"/>
       <c r="B95" s="34"/>
       <c r="C95" s="10" t="s">
         <v>141</v>
@@ -9182,7 +9182,7 @@
       <c r="E95" s="11"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A96" s="172"/>
+      <c r="A96" s="179"/>
       <c r="B96" s="34"/>
       <c r="C96" s="10" t="s">
         <v>142</v>
@@ -9191,7 +9191,7 @@
       <c r="E96" s="11"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" s="172"/>
+      <c r="A97" s="179"/>
       <c r="B97" s="34"/>
       <c r="C97" s="10" t="s">
         <v>143</v>
@@ -9200,7 +9200,7 @@
       <c r="E97" s="11"/>
     </row>
     <row r="98" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A98" s="172"/>
+      <c r="A98" s="179"/>
       <c r="B98" s="34"/>
       <c r="C98" s="10" t="s">
         <v>144</v>
@@ -9209,7 +9209,7 @@
       <c r="E98" s="11"/>
     </row>
     <row r="99" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A99" s="172"/>
+      <c r="A99" s="179"/>
       <c r="B99" s="36" t="s">
         <v>145</v>
       </c>
@@ -9222,7 +9222,7 @@
       <c r="E99" s="11"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100" s="172"/>
+      <c r="A100" s="179"/>
       <c r="B100" s="34"/>
       <c r="C100" s="10"/>
       <c r="D100" s="10" t="s">
@@ -9231,7 +9231,7 @@
       <c r="E100" s="11"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A101" s="172"/>
+      <c r="A101" s="179"/>
       <c r="B101" s="34"/>
       <c r="C101" s="10" t="s">
         <v>149</v>
@@ -9242,7 +9242,7 @@
       <c r="E101" s="11"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A102" s="172"/>
+      <c r="A102" s="179"/>
       <c r="B102" s="34"/>
       <c r="C102" s="10"/>
       <c r="D102" s="10" t="s">
@@ -9251,7 +9251,7 @@
       <c r="E102" s="11"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A103" s="172"/>
+      <c r="A103" s="179"/>
       <c r="B103" s="34"/>
       <c r="C103" s="10"/>
       <c r="D103" s="10" t="s">
@@ -9260,7 +9260,7 @@
       <c r="E103" s="11"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A104" s="172"/>
+      <c r="A104" s="179"/>
       <c r="B104" s="34"/>
       <c r="C104" s="10"/>
       <c r="D104" s="10" t="s">
@@ -9269,7 +9269,7 @@
       <c r="E104" s="11"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A105" s="172"/>
+      <c r="A105" s="179"/>
       <c r="B105" s="34"/>
       <c r="C105" s="10" t="s">
         <v>154</v>
@@ -9278,7 +9278,7 @@
       <c r="E105" s="11"/>
     </row>
     <row r="106" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A106" s="172"/>
+      <c r="A106" s="179"/>
       <c r="B106" s="34"/>
       <c r="C106" s="10" t="s">
         <v>155</v>
@@ -9287,7 +9287,7 @@
       <c r="E106" s="11"/>
     </row>
     <row r="107" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A107" s="172"/>
+      <c r="A107" s="179"/>
       <c r="B107" s="34"/>
       <c r="C107" s="10" t="s">
         <v>156</v>
@@ -9296,7 +9296,7 @@
       <c r="E107" s="11"/>
     </row>
     <row r="108" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A108" s="172"/>
+      <c r="A108" s="179"/>
       <c r="B108" s="34"/>
       <c r="C108" s="10" t="s">
         <v>157</v>
@@ -9305,7 +9305,7 @@
       <c r="E108" s="11"/>
     </row>
     <row r="109" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A109" s="172"/>
+      <c r="A109" s="179"/>
       <c r="B109" s="34"/>
       <c r="C109" s="10" t="s">
         <v>158</v>
@@ -9314,7 +9314,7 @@
       <c r="E109" s="11"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A110" s="172"/>
+      <c r="A110" s="179"/>
       <c r="B110" s="36" t="s">
         <v>159</v>
       </c>
@@ -9325,7 +9325,7 @@
       <c r="E110" s="11"/>
     </row>
     <row r="111" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A111" s="172"/>
+      <c r="A111" s="179"/>
       <c r="B111" s="34"/>
       <c r="C111" s="10" t="s">
         <v>161</v>
@@ -9336,7 +9336,7 @@
       <c r="E111" s="11"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112" s="172"/>
+      <c r="A112" s="179"/>
       <c r="B112" s="34"/>
       <c r="C112" s="10"/>
       <c r="D112" s="10" t="s">
@@ -9345,7 +9345,7 @@
       <c r="E112" s="11"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A113" s="172"/>
+      <c r="A113" s="179"/>
       <c r="B113" s="36" t="s">
         <v>164</v>
       </c>
@@ -9356,7 +9356,7 @@
       <c r="E113" s="11"/>
     </row>
     <row r="114" spans="1:5" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A114" s="172"/>
+      <c r="A114" s="179"/>
       <c r="B114" s="34"/>
       <c r="C114" s="10" t="s">
         <v>166</v>
@@ -9365,7 +9365,7 @@
       <c r="E114" s="11"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A115" s="172"/>
+      <c r="A115" s="179"/>
       <c r="B115" s="36" t="s">
         <v>167</v>
       </c>
@@ -9378,7 +9378,7 @@
       <c r="E115" s="11"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A116" s="172"/>
+      <c r="A116" s="179"/>
       <c r="B116" s="34"/>
       <c r="C116" s="10"/>
       <c r="D116" s="10" t="s">
@@ -9387,7 +9387,7 @@
       <c r="E116" s="11"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A117" s="172"/>
+      <c r="A117" s="179"/>
       <c r="B117" s="34"/>
       <c r="C117" s="10"/>
       <c r="D117" s="10" t="s">
@@ -9396,7 +9396,7 @@
       <c r="E117" s="11"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A118" s="172"/>
+      <c r="A118" s="179"/>
       <c r="B118" s="34"/>
       <c r="C118" s="10" t="s">
         <v>172</v>
@@ -9405,7 +9405,7 @@
       <c r="E118" s="11"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A119" s="172"/>
+      <c r="A119" s="179"/>
       <c r="B119" s="34"/>
       <c r="C119" s="10" t="s">
         <v>173</v>
@@ -9416,7 +9416,7 @@
       <c r="E119" s="11"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A120" s="172"/>
+      <c r="A120" s="179"/>
       <c r="B120" s="34"/>
       <c r="C120" s="10"/>
       <c r="D120" s="10" t="s">
@@ -9425,7 +9425,7 @@
       <c r="E120" s="11"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A121" s="172"/>
+      <c r="A121" s="179"/>
       <c r="B121" s="34"/>
       <c r="C121" s="10"/>
       <c r="D121" s="10" t="s">
@@ -9434,7 +9434,7 @@
       <c r="E121" s="11"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A122" s="172"/>
+      <c r="A122" s="179"/>
       <c r="B122" s="34"/>
       <c r="C122" s="10" t="s">
         <v>177</v>
@@ -9443,7 +9443,7 @@
       <c r="E122" s="11"/>
     </row>
     <row r="123" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="173"/>
+      <c r="A123" s="180"/>
       <c r="B123" s="33"/>
       <c r="C123" s="13" t="s">
         <v>178</v>
@@ -9466,17 +9466,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A43:A49"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A75"/>
+    <mergeCell ref="A76:A123"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A43:A49"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A75"/>
-    <mergeCell ref="A76:A123"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>